<commit_message>
updated the cap rate
</commit_message>
<xml_diff>
--- a/Toronto vs montreal.xlsx
+++ b/Toronto vs montreal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c0727c29a80b979/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\progs\montrealvstorontoxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4206F978-6163-48A3-B3D2-7FA217D7EB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13282678-1802-4C7A-997C-39574B66900C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{788DD19D-EB1A-4A51-9072-7C1BF453AA3F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Price of the average Property in Montreal given an average per month rent of 698 Dollars using the perpetuity formual with a 1.5 growth rate</t>
   </si>
@@ -113,6 +113,30 @@
   </si>
   <si>
     <t>6% more</t>
+  </si>
+  <si>
+    <t>Time needed to accumulate down payment</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assuming a salary of 100K then 60K disposable income. 5000 dollars a month. 1000 dollars expenses. 1194 rent 500 dollars incidents so =&gt; </t>
+  </si>
+  <si>
+    <t>Montreal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assuming a salary of 100K then 60K disposable income. 5000 dollars a month. 1000 dollars expenses. 698 rent 500 dollars incidents so =&gt; </t>
+  </si>
+  <si>
+    <t>time to save</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>takes twice as long for toronto than montreal</t>
   </si>
 </sst>
 </file>
@@ -469,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30E55A0-D45D-412C-94CC-7FB3CFDF04B6}">
-  <dimension ref="A1:Y17"/>
+  <dimension ref="A1:Y22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="H7" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,8 +511,8 @@
         <v>0</v>
       </c>
       <c r="P1">
-        <f>698*12/(0.032-0.015)</f>
-        <v>492705.88235294115</v>
+        <f>698*12/(0.06-0.02)</f>
+        <v>209400.00000000003</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.35">
@@ -496,8 +520,8 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <f>1194*12/(0.032-0.015)</f>
-        <v>842823.5294117647</v>
+        <f>1194*12/(0.06-0.02)</f>
+        <v>358200.00000000006</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
@@ -517,39 +541,39 @@
       </c>
       <c r="H6">
         <f>PMT(0.032,25,-P1*0.8)/12</f>
-        <v>1928.6204509225847</v>
+        <v>819.6636916420988</v>
       </c>
       <c r="I6">
         <f>H6*12</f>
-        <v>23143.445411071018</v>
+        <v>9835.9642997051851</v>
       </c>
       <c r="J6" t="s">
         <v>3</v>
       </c>
       <c r="L6">
         <f>20%*P1</f>
-        <v>98541.176470588238</v>
+        <v>41880.000000000007</v>
       </c>
       <c r="N6" t="s">
         <v>4</v>
       </c>
       <c r="Q6">
         <f>P1*1.5</f>
-        <v>739058.82352941169</v>
+        <v>314100.00000000006</v>
       </c>
       <c r="S6" t="s">
         <v>5</v>
       </c>
       <c r="V6">
         <f>P1-Montreal!E11-L6</f>
-        <v>170136.15430318541</v>
+        <v>72307.865578853845</v>
       </c>
       <c r="X6" t="s">
         <v>13</v>
       </c>
       <c r="Y6">
         <f>Q6-V6</f>
-        <v>568922.66922622628</v>
+        <v>241792.13442114621</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
@@ -561,39 +585,39 @@
       </c>
       <c r="H7" s="1">
         <f>PMT(0.032,25,-P3*0.8)/12</f>
-        <v>3299.1014590280324</v>
+        <v>1402.1181200869139</v>
       </c>
       <c r="I7" s="1">
         <f>H7*12</f>
-        <v>39589.217508336391</v>
+        <v>16825.417441042966</v>
       </c>
       <c r="J7" t="s">
         <v>3</v>
       </c>
       <c r="L7">
         <f>P3*20%</f>
-        <v>168564.70588235295</v>
+        <v>71640.000000000015</v>
       </c>
       <c r="N7" t="s">
         <v>4</v>
       </c>
       <c r="Q7">
         <f>P3*2.25</f>
-        <v>1896352.9411764706</v>
+        <v>805950.00000000012</v>
       </c>
       <c r="S7" t="s">
         <v>5</v>
       </c>
       <c r="V7">
         <f>P3-Toronto!E11-L7</f>
-        <v>291035.19804871548</v>
+        <v>123689.95917070417</v>
       </c>
       <c r="X7" t="s">
         <v>13</v>
       </c>
       <c r="Y7">
         <f>Q7-V7</f>
-        <v>1605317.7431277551</v>
+        <v>682260.04082929599</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.35">
@@ -605,21 +629,21 @@
       </c>
       <c r="F9">
         <f>L7-L6</f>
-        <v>70023.529411764714</v>
+        <v>29760.000000000007</v>
       </c>
       <c r="H9" t="s">
         <v>23</v>
       </c>
       <c r="K9" s="1">
         <f>H7-H6</f>
-        <v>1370.4810081054477</v>
+        <v>582.45442844481511</v>
       </c>
       <c r="M9" t="s">
         <v>24</v>
       </c>
       <c r="N9" s="1">
         <f>F9+K9*12*10</f>
-        <v>234481.25038441847</v>
+        <v>99654.531413377816</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.35">
@@ -628,7 +652,7 @@
       </c>
       <c r="F10" s="1">
         <f>N9*100000/60000</f>
-        <v>390802.08397403074</v>
+        <v>166090.88568896303</v>
       </c>
       <c r="H10" t="s">
         <v>15</v>
@@ -650,7 +674,7 @@
       </c>
       <c r="G14" s="1">
         <f>(F10+Y6)*0.93</f>
-        <v>892544.02047623903</v>
+        <v>379331.20870240161</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>25</v>
@@ -662,16 +686,68 @@
       </c>
       <c r="G15">
         <f>Y7</f>
-        <v>1605317.7431277551</v>
-      </c>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.35">
+        <v>682260.04082929599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="G17" s="1">
         <f>G15-G14</f>
-        <v>712773.72265151609</v>
+        <v>302928.83212689438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21">
+        <f>5000-(1000+1194+500)</f>
+        <v>2306</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>31</v>
+      </c>
+      <c r="S21">
+        <f>L7/O21/12</f>
+        <v>2.5888985255854298</v>
+      </c>
+      <c r="T21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="O22">
+        <f>5000-(1000+698+500)</f>
+        <v>2802</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>31</v>
+      </c>
+      <c r="S22">
+        <f>L6/O22/12</f>
+        <v>1.2455389007851536</v>
+      </c>
+      <c r="T22" t="s">
+        <v>32</v>
+      </c>
+      <c r="V22" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -684,7 +760,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,15 +784,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C2">
         <f>B2*0.032</f>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D2">
         <f>B2-C2</f>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -724,15 +801,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C26" si="0">B3*0.032</f>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D26" si="1">B3-C3</f>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -740,15 +818,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -756,15 +835,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -772,15 +852,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -788,15 +869,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -804,15 +886,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -820,15 +903,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -836,15 +920,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -852,19 +937,20 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
       <c r="E11">
         <f>SUM(D2:D11)</f>
-        <v>224028.55157916748</v>
+        <v>95212.134421146184</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -872,15 +958,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -888,15 +975,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -904,15 +992,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -920,15 +1009,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -936,15 +1026,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -952,15 +1043,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -968,15 +1060,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -984,15 +1077,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -1000,15 +1094,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1016,15 +1111,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1032,15 +1128,16 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -1048,15 +1145,16 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1064,15 +1162,16 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -1080,15 +1179,16 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -1096,15 +1196,16 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>23143.445411071018</v>
+        <f>Total!$I$6</f>
+        <v>9835.9642997051851</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>740.59025315427255</v>
+        <v>314.75085759056594</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>22402.855157916743</v>
+        <v>9521.2134421146184</v>
       </c>
     </row>
   </sheetData>
@@ -1116,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4BC293-CB2B-4641-BD17-AA508900ED90}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1141,404 +1242,429 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>39589.217508336391</v>
+      <c r="B2" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C2">
         <f>B2*0.032</f>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D2">
         <f>B2-C2</f>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>39589.217508336391</v>
+      <c r="B3" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C26" si="0">B3*0.032</f>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D26" si="1">B3-C3</f>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>39589.217508336391</v>
+      <c r="B4" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>39589.217508336391</v>
+      <c r="B5" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>39589.217508336391</v>
+      <c r="B6" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>39589.217508336391</v>
+      <c r="B7" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>39589.217508336391</v>
+      <c r="B8" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>39589.217508336391</v>
+      <c r="B9" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>39589.217508336391</v>
+      <c r="B10" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>39589.217508336391</v>
+      <c r="B11" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
       <c r="E11">
         <f>SUM(D2:D11)</f>
-        <v>383223.62548069627</v>
+        <v>162870.04082929587</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>39589.217508336391</v>
+      <c r="B12" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>39589.217508336391</v>
+      <c r="B13" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>39589.217508336391</v>
+      <c r="B14" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>39589.217508336391</v>
+      <c r="B15" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>39589.217508336391</v>
+      <c r="B16" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>39589.217508336391</v>
+      <c r="B17" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>39589.217508336391</v>
+      <c r="B18" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>39589.217508336391</v>
+      <c r="B19" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>39589.217508336391</v>
+      <c r="B20" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>39589.217508336391</v>
+      <c r="B21" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>39589.217508336391</v>
+      <c r="B22" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23">
-        <v>39589.217508336391</v>
+      <c r="B23" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>39589.217508336391</v>
+      <c r="B24" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>39589.217508336391</v>
+      <c r="B25" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>39589.217508336391</v>
+      <c r="B26" s="1">
+        <f>Total!$I$7</f>
+        <v>16825.417441042966</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>1266.8549602667645</v>
+        <v>538.4133581133749</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>38322.362548069628</v>
+        <v>16287.00408292959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>